<commit_message>
almost finished all models
</commit_message>
<xml_diff>
--- a/Output/AllModels_final_with_plan_and_barriers12000.xlsx
+++ b/Output/AllModels_final_with_plan_and_barriers12000.xlsx
@@ -365,7 +365,7 @@
     <t xml:space="preserve">[0.53,    1.20]</t>
   </si>
   <si>
-    <t xml:space="preserve">Daily weartime</t>
+    <t xml:space="preserve">Daily wear time</t>
   </si>
   <si>
     <t xml:space="preserve">1.00***</t>
@@ -623,7 +623,7 @@
     <t xml:space="preserve">[0.38,    2.52]</t>
   </si>
   <si>
-    <t xml:space="preserve">Mean weartime</t>
+    <t xml:space="preserve">Mean wear time</t>
   </si>
   <si>
     <t xml:space="preserve">1.00*</t>

</xml_diff>